<commit_message>
first try on rubrics
</commit_message>
<xml_diff>
--- a/exercises/2020-21/oversigt.xlsx
+++ b/exercises/2020-21/oversigt.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP.git/exercises/2020-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9D6EB12-C5EB-C540-8286-E6A2FE903948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE131013-A255-004A-B241-A27B62984366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="940" windowWidth="24800" windowHeight="17060" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
+    <workbookView xWindow="28320" yWindow="5400" windowWidth="25600" windowHeight="12860" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Opgave</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Emne</t>
   </si>
   <si>
-    <t>Fokus</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
@@ -101,12 +98,6 @@
     <t>Eksempler</t>
   </si>
   <si>
-    <t>F#, Compiler vs. fortolker, tegnsæt, simple typer</t>
-  </si>
-  <si>
-    <t>Scratch, Lav et spil, aflever en opgave, tale om programmer</t>
-  </si>
-  <si>
     <t>Paradigme</t>
   </si>
   <si>
@@ -122,16 +113,121 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Funktioner, løkker og kommentarer</t>
-  </si>
-  <si>
-    <t>Krav til beståelse</t>
-  </si>
-  <si>
-    <t>Skal: lave et spil, lave en pdf fra LaTeX, aflevere i Absalon</t>
-  </si>
-  <si>
-    <t>Skal: lave et F# program, spil, lave en pdf fra LaTeX, aflevere i Absalon</t>
+    <t>Rubrikker</t>
+  </si>
+  <si>
+    <t>Fungerende spil i Scratch</t>
+  </si>
+  <si>
+    <t>Lille rapport i LateX, der oversætter og producerer en pdf. Skal indeholde en figur</t>
+  </si>
+  <si>
+    <t>Aflevering gennemført som gruppe i Absalon</t>
+  </si>
+  <si>
+    <t>Kende forskel på fortolker og compiler, lave et fortolket og et compilet program.</t>
+  </si>
+  <si>
+    <t>Demonstrere evne til at arbejde med strenge inkl. danske bogstaver</t>
+  </si>
+  <si>
+    <t>Fungerende programmer med løkker både som for- og while-løkker og kunne implementere en for-løkke som en while-løkke. Lave en dobbelt for-løkke.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skrive programmer med funktioner. </t>
+  </si>
+  <si>
+    <t>Læse input fra tastaturet</t>
+  </si>
+  <si>
+    <t>Producere output på skærmen med printf og styrre formatteringen.</t>
+  </si>
+  <si>
+    <t>Gruppere funktioner i moduler</t>
+  </si>
+  <si>
+    <t>Gennemføre en afprøvning</t>
+  </si>
+  <si>
+    <t>Dokumentere funktioner i kode og med kommentarstandarden</t>
+  </si>
+  <si>
+    <t>Oprette, gennemløbe og lave beregninger med lister</t>
+  </si>
+  <si>
+    <t>Skrive funktioner, som bruger patterns til behandling af simple typer og lister</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Martin overvejer rækkefølgen for lister, rekursion og patterns</t>
+  </si>
+  <si>
+    <t>Oprette, gennemløbe og ændre arrays. Kunne beskrive forskellen mellem lister og arrays</t>
+  </si>
+  <si>
+    <t>Gemmenløbe en liste imperativt og rekursivt med patterns, og forklare fordele og ulemper ved de 2 tilgange</t>
+  </si>
+  <si>
+    <t>Løse et problem vha. rekurssion</t>
+  </si>
+  <si>
+    <t>Løse et større programmeringsproblem vha. rekursion, lister og patterns</t>
+  </si>
+  <si>
+    <t>Kalde og skrive funktioner, som tager funktioner som argument</t>
+  </si>
+  <si>
+    <t>Bruge map, fold og foldback på lister</t>
+  </si>
+  <si>
+    <t>Skrive en rekursiv funktion og forklare forskellen på alm. og halerekurssion</t>
+  </si>
+  <si>
+    <t>Håndtere fejl vha. untagelser fra systemet og ved selv at kaste untagelser</t>
+  </si>
+  <si>
+    <t>Læse og skrive til en fil</t>
+  </si>
+  <si>
+    <t>Læse fra internettet</t>
+  </si>
+  <si>
+    <t>Skrive en klasse med metoder og properties</t>
+  </si>
+  <si>
+    <t>Skrive en white- og en black-box test af en klasse</t>
+  </si>
+  <si>
+    <t>Demonstrere brug af "programmer-baglæns" metoden</t>
+  </si>
+  <si>
+    <t>Skrive klasser med nedarvning</t>
+  </si>
+  <si>
+    <t>Lav et objektorienteret design med uml diagram</t>
+  </si>
+  <si>
+    <t>Lav en klasse med statiske metoder og properties</t>
+  </si>
+  <si>
+    <t>Udvide et eksisterende design</t>
+  </si>
+  <si>
+    <t>Udvide et eksisterend objekt-orienteret program</t>
+  </si>
+  <si>
+    <t>Programmer en grafisk brugergrænseflade</t>
+  </si>
+  <si>
+    <t>Bruge callback funktioner til at styre brugerinteraktion</t>
+  </si>
+  <si>
+    <t>ditto</t>
+  </si>
+  <si>
+    <t>ditto, her skal tilføjes noget med typer</t>
   </si>
 </sst>
 </file>
@@ -167,10 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,24 +585,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BE6506-6C30-F84B-A24A-3A8F093A9ACA}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.5" customWidth="1"/>
+    <col min="7" max="9" width="32.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -511,275 +613,377 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B15" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>2.5</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <f>SUM(D3:D15)</f>

</xml_diff>

<commit_message>
working on new worksheets. 1g and 2i out for review
</commit_message>
<xml_diff>
--- a/exercises/2020-21/oversigt.xlsx
+++ b/exercises/2020-21/oversigt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP.git/exercises/2020-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE131013-A255-004A-B241-A27B62984366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A994B1F-6E57-AF4B-985A-ABC48AF6F2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28320" yWindow="5400" windowWidth="25600" windowHeight="12860" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
+    <workbookView xWindow="4700" yWindow="460" windowWidth="21460" windowHeight="17540" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
     <t>Opgave</t>
   </si>
@@ -228,6 +228,33 @@
   </si>
   <si>
     <t>ditto, her skal tilføjes noget med typer</t>
+  </si>
+  <si>
+    <t>Rapportform</t>
+  </si>
+  <si>
+    <t>opgave.pdf</t>
+  </si>
+  <si>
+    <t>udvidet kommentarer</t>
+  </si>
+  <si>
+    <t>rapport.pdf</t>
+  </si>
+  <si>
+    <t>Introtekst</t>
+  </si>
+  <si>
+    <t>Velkommen</t>
+  </si>
+  <si>
+    <t>Velkommen-kortform</t>
+  </si>
+  <si>
+    <t>Rapport</t>
+  </si>
+  <si>
+    <t>Afslutning</t>
   </si>
 </sst>
 </file>
@@ -585,27 +612,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BE6506-6C30-F84B-A24A-3A8F093A9ACA}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="7" max="9" width="32.83203125" style="2" customWidth="1"/>
+    <col min="7" max="11" width="32.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -630,11 +663,11 @@
       <c r="I2" s="2">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -659,8 +692,14 @@
       <c r="I3" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
@@ -683,8 +722,14 @@
       <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="J4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B15" si="0">B4+1</f>
         <v>3</v>
@@ -710,8 +755,14 @@
       <c r="I5" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -737,8 +788,14 @@
       <c r="I6" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="J6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -765,10 +822,16 @@
         <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -795,10 +858,16 @@
         <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -819,10 +888,16 @@
         <v>46</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -845,8 +920,14 @@
       <c r="H10" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="J10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -872,8 +953,14 @@
       <c r="I11" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -899,8 +986,14 @@
       <c r="I12" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -926,8 +1019,14 @@
       <c r="I13" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -950,8 +1049,14 @@
       <c r="H14" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="J14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -974,8 +1079,14 @@
       <c r="H15" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
assignment 4 reday for proofreading
</commit_message>
<xml_diff>
--- a/exercises/2020-21/oversigt.xlsx
+++ b/exercises/2020-21/oversigt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP.git/exercises/2020-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AF6E84-7130-6646-A6B5-CEABA65217DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E7BD4-9888-5542-901B-F1B0A47D22F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="2880" windowWidth="32340" windowHeight="16920" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>Gruppere funktioner i moduler</t>
   </si>
   <si>
-    <t>Gennemføre en afprøvning</t>
-  </si>
-  <si>
     <t>Dokumentere funktioner i kode og med kommentarstandarden</t>
   </si>
   <si>
@@ -260,17 +257,27 @@
     <t>4</t>
   </si>
   <si>
-    <t>Dokumentere et program via kommentarer i koden.</t>
+    <t>Gennemføre en whitebox og blackbox afprøvning</t>
+  </si>
+  <si>
+    <t>Kunne skrive og bruge en signaturfil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,12 +303,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,7 +631,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,10 +648,10 @@
         <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -670,10 +680,10 @@
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -702,10 +712,10 @@
         <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -726,16 +736,16 @@
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -762,16 +772,16 @@
         <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -795,16 +805,16 @@
         <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="102" x14ac:dyDescent="0.2">
@@ -825,22 +835,22 @@
         <v>12</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -861,25 +871,25 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="K8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -897,16 +907,16 @@
         <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -927,16 +937,16 @@
         <v>14</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -957,19 +967,19 @@
         <v>15</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -990,19 +1000,19 @@
         <v>16</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="K12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -1023,19 +1033,19 @@
         <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -1056,16 +1066,16 @@
         <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -1086,16 +1096,16 @@
         <v>19</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="K15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
first take on 5g
</commit_message>
<xml_diff>
--- a/exercises/2020-21/oversigt.xlsx
+++ b/exercises/2020-21/oversigt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP.git/exercises/2020-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15EB1C6-6528-BD46-B38A-2E772A47ED20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6658476-6C17-9C40-BB14-9638083F852C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20020" windowHeight="17540" xr2:uid="{6E09FBD5-B6B9-8445-8CDF-5C882526F0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BE6506-6C30-F84B-A24A-3A8F093A9ACA}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>